<commit_message>
[Report] Transformed graphs into vector images
</commit_message>
<xml_diff>
--- a/report/Benchmark_message_handling.xlsx
+++ b/report/Benchmark_message_handling.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Mean RTT</t>
   </si>
@@ -42,6 +42,12 @@
   </si>
   <si>
     <t>total incoming messages / second</t>
+  </si>
+  <si>
+    <t>min error</t>
+  </si>
+  <si>
+    <t>max error</t>
   </si>
 </sst>
 </file>
@@ -181,7 +187,7 @@
           <c:yMode val="edge"/>
           <c:x val="9.3544618536861676E-2"/>
           <c:y val="0.19618923923257064"/>
-          <c:w val="0.79908566251607083"/>
+          <c:w val="0.87966303425615811"/>
           <c:h val="0.59542744470862019"/>
         </c:manualLayout>
       </c:layout>
@@ -1078,8 +1084,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1232428144"/>
-        <c:axId val="1232429776"/>
+        <c:axId val="-1871916288"/>
+        <c:axId val="-1871919552"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1224,7 +1230,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1232428144"/>
+        <c:axId val="-1871916288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1337,7 +1343,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1232429776"/>
+        <c:crossAx val="-1871919552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1345,12 +1351,26 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1232429776"/>
+        <c:axId val="-1871919552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1444,7 +1464,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1232428144"/>
+        <c:crossAx val="-1871916288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2548,8 +2568,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1350896496"/>
-        <c:axId val="1350889424"/>
+        <c:axId val="-1871924992"/>
+        <c:axId val="-1871924448"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -2694,7 +2714,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1350896496"/>
+        <c:axId val="-1871924992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2807,7 +2827,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1350889424"/>
+        <c:crossAx val="-1871924448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2815,12 +2835,26 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1350889424"/>
+        <c:axId val="-1871924448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -2914,7 +2948,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1350896496"/>
+        <c:crossAx val="-1871924992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3828,11 +3862,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1350887792"/>
-        <c:axId val="1350898128"/>
+        <c:axId val="-1924480880"/>
+        <c:axId val="-1924488496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1350887792"/>
+        <c:axId val="-1924480880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3897,7 +3931,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1350898128"/>
+        <c:crossAx val="-1924488496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3905,7 +3939,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1350898128"/>
+        <c:axId val="-1924488496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3945,7 +3979,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1350887792"/>
+        <c:crossAx val="-1924480880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4066,6 +4100,162 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Blad1!$G$26:$G$45</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="20"/>
+                  <c:pt idx="0">
+                    <c:v>0.5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.8</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.9</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.8</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.3</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>2.5</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>2.6</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>9.3000000000000007</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>9.5</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>12.9</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>10.3</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>17.8</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>29.3</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>48.2</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>54.1</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>10.9</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Blad1!$F$26:$F$45</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="20"/>
+                  <c:pt idx="0">
+                    <c:v>0.3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.1</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.5</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.1</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>1.2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>1.2</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>2.7</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>12.2</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>11.9</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>8.1</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>10.8</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>19.3</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>20</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>24.1</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>40.9</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:numRef>
               <c:f>Blad1!$C$26:$C$45</c:f>
@@ -4243,11 +4433,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="1228991312"/>
-        <c:axId val="1228991856"/>
+        <c:axId val="-1924479792"/>
+        <c:axId val="-1924478160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1228991312"/>
+        <c:axId val="-1924479792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4346,7 +4536,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1228991856"/>
+        <c:crossAx val="-1924478160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4354,12 +4544,25 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1228991856"/>
+        <c:axId val="-1924478160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -4447,7 +4650,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1228991312"/>
+        <c:crossAx val="-1924479792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6179,8 +6382,8 @@
       <xdr:rowOff>106858</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>585725</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>242455</xdr:colOff>
       <xdr:row>78</xdr:row>
       <xdr:rowOff>120609</xdr:rowOff>
     </xdr:to>
@@ -6203,16 +6406,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>28961</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1102687</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>145677</xdr:rowOff>
+      <xdr:rowOff>111040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>672352</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>58819</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>731371</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>86590</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6263,16 +6466,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>894520</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>780220</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>5195</xdr:rowOff>
+      <xdr:rowOff>164635</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>600808</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>486508</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>159440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6624,8 +6827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:AF45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView tabSelected="1" topLeftCell="D19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7935,6 +8138,12 @@
       <c r="E25" t="s">
         <v>0</v>
       </c>
+      <c r="F25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="26" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C26">
@@ -7943,6 +8152,16 @@
       <c r="E26" s="2">
         <v>32.1</v>
       </c>
+      <c r="F26">
+        <v>0.3</v>
+      </c>
+      <c r="G26">
+        <v>0.5</v>
+      </c>
+      <c r="H26">
+        <f>F26+G26</f>
+        <v>0.8</v>
+      </c>
     </row>
     <row r="27" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C27">
@@ -7951,6 +8170,16 @@
       <c r="E27" s="2">
         <v>32</v>
       </c>
+      <c r="F27">
+        <v>0.1</v>
+      </c>
+      <c r="G27">
+        <v>0.8</v>
+      </c>
+      <c r="H27">
+        <f t="shared" ref="H27:H45" si="8">F27+G27</f>
+        <v>0.9</v>
+      </c>
     </row>
     <row r="28" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C28">
@@ -7959,6 +8188,16 @@
       <c r="E28" s="2">
         <v>32.5</v>
       </c>
+      <c r="F28">
+        <v>0.3</v>
+      </c>
+      <c r="G28">
+        <v>0.9</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="8"/>
+        <v>1.2</v>
+      </c>
     </row>
     <row r="29" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C29">
@@ -7967,6 +8206,16 @@
       <c r="E29" s="2">
         <v>32.200000000000003</v>
       </c>
+      <c r="F29">
+        <v>0.4</v>
+      </c>
+      <c r="G29">
+        <v>0.4</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="8"/>
+        <v>0.8</v>
+      </c>
     </row>
     <row r="30" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C30">
@@ -7975,6 +8224,16 @@
       <c r="E30" s="2">
         <v>32.700000000000003</v>
       </c>
+      <c r="F30">
+        <v>0.5</v>
+      </c>
+      <c r="G30">
+        <v>0.2</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="8"/>
+        <v>0.7</v>
+      </c>
     </row>
     <row r="31" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C31">
@@ -7983,6 +8242,16 @@
       <c r="E31" s="2">
         <v>32.700000000000003</v>
       </c>
+      <c r="F31">
+        <v>0.3</v>
+      </c>
+      <c r="G31">
+        <v>0.3</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="8"/>
+        <v>0.6</v>
+      </c>
     </row>
     <row r="32" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C32">
@@ -7991,24 +8260,54 @@
       <c r="E32" s="2">
         <v>32.1</v>
       </c>
+      <c r="F32">
+        <v>0.4</v>
+      </c>
+      <c r="G32">
+        <v>0.8</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="8"/>
+        <v>1.2000000000000002</v>
+      </c>
     </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C33">
         <v>4000</v>
       </c>
       <c r="E33" s="2">
         <v>32</v>
       </c>
+      <c r="F33">
+        <v>0.1</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="8"/>
+        <v>1.1000000000000001</v>
+      </c>
     </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C34">
         <v>4500</v>
       </c>
       <c r="E34" s="2">
         <v>32.9</v>
       </c>
+      <c r="F34">
+        <v>1.2</v>
+      </c>
+      <c r="G34">
+        <v>0.3</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="8"/>
+        <v>1.5</v>
+      </c>
     </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C35">
         <v>5000</v>
       </c>
@@ -8016,40 +8315,90 @@
         <f>AVERAGE(L18,M17,N14,O9,P6)</f>
         <v>39.980000000000004</v>
       </c>
+      <c r="F35">
+        <v>1.2</v>
+      </c>
+      <c r="G35">
+        <v>2.5</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="8"/>
+        <v>3.7</v>
+      </c>
     </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C36">
         <v>5500</v>
       </c>
       <c r="E36" s="2">
         <v>42</v>
       </c>
+      <c r="F36">
+        <v>2</v>
+      </c>
+      <c r="G36">
+        <v>2.6</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="8"/>
+        <v>4.5999999999999996</v>
+      </c>
     </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C37">
         <v>6000</v>
       </c>
       <c r="E37" s="2">
         <v>44</v>
       </c>
+      <c r="F37">
+        <v>2.7</v>
+      </c>
+      <c r="G37">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
     </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C38">
         <v>6500</v>
       </c>
       <c r="E38" s="2">
         <v>55</v>
       </c>
+      <c r="F38">
+        <v>12.2</v>
+      </c>
+      <c r="G38">
+        <v>9.5</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="8"/>
+        <v>21.7</v>
+      </c>
     </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C39">
         <v>7000</v>
       </c>
       <c r="E39" s="2">
         <v>60</v>
       </c>
+      <c r="F39">
+        <v>11.9</v>
+      </c>
+      <c r="G39">
+        <v>12.9</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="8"/>
+        <v>24.8</v>
+      </c>
     </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C40">
         <v>7500</v>
       </c>
@@ -8057,46 +8406,106 @@
         <f>AVERAGE(L19,N15,O11,P7,R5)</f>
         <v>65.42</v>
       </c>
+      <c r="F40">
+        <v>8.1</v>
+      </c>
+      <c r="G40">
+        <v>10.3</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="8"/>
+        <v>18.399999999999999</v>
+      </c>
     </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C41">
         <v>8000</v>
       </c>
       <c r="E41" s="2">
         <v>70</v>
       </c>
+      <c r="F41">
+        <v>10.8</v>
+      </c>
+      <c r="G41">
+        <v>17.8</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="8"/>
+        <v>28.6</v>
+      </c>
     </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C42">
         <v>8500</v>
       </c>
       <c r="E42" s="2">
         <v>90</v>
       </c>
+      <c r="F42">
+        <v>19.3</v>
+      </c>
+      <c r="G42">
+        <v>29.3</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="8"/>
+        <v>48.6</v>
+      </c>
     </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C43">
         <v>9000</v>
       </c>
       <c r="E43" s="2">
         <v>107</v>
       </c>
+      <c r="F43">
+        <v>20</v>
+      </c>
+      <c r="G43">
+        <v>48.2</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="8"/>
+        <v>68.2</v>
+      </c>
     </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C44">
         <v>9500</v>
       </c>
       <c r="E44" s="2">
         <v>142</v>
       </c>
+      <c r="F44">
+        <v>24.1</v>
+      </c>
+      <c r="G44">
+        <v>54.1</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="8"/>
+        <v>78.2</v>
+      </c>
     </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C45">
         <v>10000</v>
       </c>
       <c r="E45" s="2">
         <f>AVERAGE(L20,M18,N16,O14,P8,Q6)</f>
         <v>185.65</v>
+      </c>
+      <c r="F45">
+        <v>40.9</v>
+      </c>
+      <c r="G45">
+        <v>10.9</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="8"/>
+        <v>51.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>